<commit_message>
Add manual testing guide for convalidation system
Added GUIA_PRUEBAS_MANUALES.md with detailed manual test cases, prerequisites, evidence structure, and troubleshooting steps for the convalidation system workflows (HU-001 and HU-005). Also updated Registro_Horas_Proyecto.xlsx with new data.
</commit_message>
<xml_diff>
--- a/registro-trabajo/Registro_Horas_Proyecto.xlsx
+++ b/registro-trabajo/Registro_Horas_Proyecto.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\OneDrive\Escritorio\Uni2025\Practica\Proyecto-n8n-main\registro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\OneDrive\Escritorio\Uni2025\Practica\Convalidacion-Academica\registro-trabajo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322D6FA0-F6B0-4EB2-8541-0F0EDE3360B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917F184B-E7AC-4D8F-935D-10E1231FFF50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registro Diario" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
   <si>
     <t>Fecha</t>
   </si>
@@ -140,13 +140,67 @@
   </si>
   <si>
     <t>Investigacion</t>
+  </si>
+  <si>
+    <t>Planificacion Inicial HU005: Analisis de requisitos y diseño de templates</t>
+  </si>
+  <si>
+    <t>Desarrollo de 4 templates HTML para notificaciones de error</t>
+  </si>
+  <si>
+    <t>Desarrollo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuracion nodo Webhook HU-005 en n8n </t>
+  </si>
+  <si>
+    <t>Implementacion de validaciones de entrada (Function-ValidarEntrada)</t>
+  </si>
+  <si>
+    <t>Configuracion SMTP Gmail para envio de emails</t>
+  </si>
+  <si>
+    <t>Desarrollo de lógica de selección de templates (switch 4 casos)</t>
+  </si>
+  <si>
+    <t>Configuración nodo Email-Correccion con templates HTML</t>
+  </si>
+  <si>
+    <t>Pruebas unitarias de 4 templates (TC1.1-TC1.4)</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Pruebas de validación de errores (TC4.1-TC4.5)</t>
+  </si>
+  <si>
+    <t>Documentación técnica: HU-05_FICHA_TECNICA.md</t>
+  </si>
+  <si>
+    <t>Documentacion</t>
+  </si>
+  <si>
+    <t>Documentación de 20 casos de prueba: HU-05_CASOS_PRUEBA.md</t>
+  </si>
+  <si>
+    <t>Documentación de resultados de pruebas: HU-05_RESULTADOS_PRUEBAS.md</t>
+  </si>
+  <si>
+    <t>Desarrollo de script automatizado de pruebas (HU-05_test.ps1)</t>
+  </si>
+  <si>
+    <t>Captura de 9 evidencias visuales (screenshots pruebas y emails)</t>
+  </si>
+  <si>
+    <t>Exportación de 30 tareas a Taiga</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,8 +227,15 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -184,6 +245,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF3F3F3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -230,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -241,14 +308,18 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -565,7 +636,7 @@
     <col min="4" max="4" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -579,305 +650,482 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="34.200000000000003" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
+    <row r="2" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="10">
         <v>45947</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="11">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
         <v>45947</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="11">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="10">
         <v>45948</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="11">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
         <v>45948</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
         <v>45949</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
         <v>45949</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="11">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="34.200000000000003" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
         <v>45950</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="11">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
         <v>45950</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="11">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="10">
         <v>45951</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="11">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="45.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
         <v>45952</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="11">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="45.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A12" s="10">
         <v>45953</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="11">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="45.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+    </row>
+    <row r="13" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="10">
         <v>45953</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="6">
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
         <v>45963</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="11">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="6">
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
         <v>45967</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="11">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="6">
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="7">
         <v>45967</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="8">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="7">
+        <v>45967</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="8">
+        <v>2</v>
+      </c>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="7">
+        <v>45968</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="8">
+        <v>3</v>
+      </c>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="7">
+        <v>45968</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="8">
+        <v>1</v>
+      </c>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
+        <v>45969</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="6">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
+        <v>45969</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
+        <v>45970</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="5">
+        <v>45970</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="5">
+        <v>45971</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="5">
+        <v>45971</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="5">
+        <v>45972</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="5">
+        <v>45972</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" s="6">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="5">
+        <v>45972</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="5">
+        <v>45973</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="6">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="5">
+        <v>45973</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="5">
+        <v>45973</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="4"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="4"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="4"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="4"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="4"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="4"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -888,7 +1136,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -969,7 +1217,7 @@
       </c>
       <c r="B2">
         <f>SUM('Registro Diario'!D2:D1000)</f>
-        <v>29.5</v>
+        <v>57.5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -978,7 +1226,7 @@
       </c>
       <c r="B3">
         <f>(B2/256)*100</f>
-        <v>11.5234375</v>
+        <v>22.4609375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>